<commit_message>
Completed Version 1: replace bury vias to micro vias
</commit_message>
<xml_diff>
--- a/Proposal/Timetable.xlsx
+++ b/Proposal/Timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pengyuan\Desktop\FYP\Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197BE647-7F0B-4768-B0F2-0235932BFC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6430E626-140D-4920-8EF7-DA74D04F2368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,7 +346,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,12 +383,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -773,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -871,9 +865,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1255,7 +1246,7 @@
   <dimension ref="B1:AM26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AP10" sqref="AP10"/>
+      <selection activeCell="AR10" sqref="AR10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1274,57 +1265,57 @@
   <sheetData>
     <row r="1" spans="2:39" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:39" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="52"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
+      <c r="AE2" s="50"/>
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="50"/>
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
+      <c r="AK2" s="50"/>
+      <c r="AL2" s="50"/>
+      <c r="AM2" s="51"/>
     </row>
     <row r="3" spans="2:39" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="61"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="3">
         <v>3</v>
       </c>
@@ -1343,13 +1334,13 @@
       <c r="J3" s="36">
         <v>8</v>
       </c>
-      <c r="K3" s="38">
+      <c r="K3" s="37">
         <v>9</v>
       </c>
       <c r="L3" s="36">
         <v>10</v>
       </c>
-      <c r="M3" s="37">
+      <c r="M3" s="36">
         <v>11</v>
       </c>
       <c r="N3" s="3">
@@ -1432,7 +1423,7 @@
       </c>
     </row>
     <row r="4" spans="2:39" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="11">
@@ -1447,17 +1438,17 @@
       <c r="H4" s="2"/>
       <c r="I4" s="24"/>
       <c r="J4" s="25"/>
-      <c r="N4" s="57" t="s">
+      <c r="N4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="65" t="s">
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="T4" s="66"/>
+      <c r="T4" s="65"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
@@ -1465,21 +1456,21 @@
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
-      <c r="AF4" s="57" t="s">
+      <c r="AF4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="58"/>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="53" t="s">
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="57"/>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="AL4" s="53"/>
-      <c r="AM4" s="54"/>
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="53"/>
     </row>
     <row r="5" spans="2:39" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="63"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="12">
         <v>2</v>
       </c>
@@ -1493,13 +1484,13 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="15"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
       <c r="U5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
@@ -1508,17 +1499,17 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
-      <c r="AF5" s="59"/>
-      <c r="AG5" s="59"/>
-      <c r="AH5" s="59"/>
-      <c r="AI5" s="59"/>
-      <c r="AJ5" s="59"/>
-      <c r="AK5" s="55"/>
-      <c r="AL5" s="55"/>
-      <c r="AM5" s="56"/>
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="54"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="55"/>
     </row>
     <row r="6" spans="2:39" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="63"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="12">
         <v>3</v>
       </c>
@@ -1530,13 +1521,13 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="67"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="66"/>
+      <c r="T6" s="66"/>
       <c r="U6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
@@ -1545,17 +1536,17 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
-      <c r="AF6" s="59"/>
-      <c r="AG6" s="59"/>
-      <c r="AH6" s="59"/>
-      <c r="AI6" s="59"/>
-      <c r="AJ6" s="59"/>
-      <c r="AK6" s="55"/>
-      <c r="AL6" s="55"/>
-      <c r="AM6" s="56"/>
+      <c r="AF6" s="58"/>
+      <c r="AG6" s="58"/>
+      <c r="AH6" s="58"/>
+      <c r="AI6" s="58"/>
+      <c r="AJ6" s="58"/>
+      <c r="AK6" s="54"/>
+      <c r="AL6" s="54"/>
+      <c r="AM6" s="55"/>
     </row>
     <row r="7" spans="2:39" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="64"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="13">
         <v>4</v>
       </c>
@@ -1567,8 +1558,8 @@
       <c r="G7" s="2"/>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="40"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="39"/>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
@@ -1594,7 +1585,7 @@
       <c r="AM7" s="19"/>
     </row>
     <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="61" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="11">
@@ -1635,7 +1626,7 @@
       <c r="AM8" s="19"/>
     </row>
     <row r="9" spans="2:39" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="63"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="12">
         <v>6</v>
       </c>
@@ -1673,7 +1664,7 @@
       <c r="AM9" s="19"/>
     </row>
     <row r="10" spans="2:39" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="64"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="13">
         <v>7</v>
       </c>
@@ -1707,7 +1698,7 @@
       <c r="AM10" s="19"/>
     </row>
     <row r="11" spans="2:39" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="12">
@@ -1743,7 +1734,7 @@
       <c r="AM11" s="19"/>
     </row>
     <row r="12" spans="2:39" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="63"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="12">
         <v>9</v>
       </c>
@@ -1779,7 +1770,7 @@
       <c r="AM12" s="19"/>
     </row>
     <row r="13" spans="2:39" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="63"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="12">
         <v>10</v>
       </c>
@@ -1813,7 +1804,7 @@
       <c r="AM13" s="19"/>
     </row>
     <row r="14" spans="2:39" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="63"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="12">
         <v>11</v>
       </c>
@@ -1847,11 +1838,11 @@
       <c r="AM14" s="19"/>
     </row>
     <row r="15" spans="2:39" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1885,11 +1876,11 @@
       <c r="AM15" s="19"/>
     </row>
     <row r="16" spans="2:39" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="43"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1927,11 +1918,11 @@
       <c r="AM16" s="20"/>
     </row>
     <row r="17" spans="2:39" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1977,11 +1968,11 @@
       <c r="AM17" s="33"/>
     </row>
     <row r="18" spans="2:39" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>

</xml_diff>